<commit_message>
Update interface, excel output and running configurations
Some updates:
1. Updated the choosing parameters interface so that the user can choose the values of some of the input.
2. Excel output now also includes different resutls in an additional excel file.
3. Modified the .mod file so that he will stop the model when the Optimality Gap is no more than 1%, making it possible to run the full dataset without problems.
</commit_message>
<xml_diff>
--- a/energy_consumption_by_yeshuv-average_consumption_times_population_per_yeshuv.xlsx
+++ b/energy_consumption_by_yeshuv-average_consumption_times_population_per_yeshuv.xlsx
@@ -8,15 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxpo\OneDrive\Desktop\OPL_solver_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BACCCA4-2031-4D5E-8327-BB0418929BCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C896B817-A14D-4759-BAE5-307747CCAE25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -3716,9 +3726,6 @@
     <t>רמות</t>
   </si>
   <si>
-    <t>תל אביב - יפו</t>
-  </si>
-  <si>
     <t>באקה אל-גרביה</t>
   </si>
   <si>
@@ -3831,6 +3838,9 @@
   </si>
   <si>
     <t>בנימינה-גבעת עדה</t>
+  </si>
+  <si>
+    <t>תל אביב-יפו</t>
   </si>
 </sst>
 </file>
@@ -4234,11 +4244,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1268"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A1241" workbookViewId="0">
+      <selection activeCell="G1254" sqref="G1254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -17764,7 +17778,7 @@
         <v>5000</v>
       </c>
       <c r="B1230" t="s">
-        <v>1231</v>
+        <v>1269</v>
       </c>
       <c r="C1230">
         <v>1175520.3857307821</v>
@@ -17775,7 +17789,7 @@
         <v>6000</v>
       </c>
       <c r="B1231" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="C1231">
         <v>64897.307112572387</v>
@@ -17786,7 +17800,7 @@
         <v>6100</v>
       </c>
       <c r="B1232" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C1232">
         <v>463949.13924563891</v>
@@ -17797,7 +17811,7 @@
         <v>6200</v>
       </c>
       <c r="B1233" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C1233">
         <v>320570.38793445402</v>
@@ -17808,7 +17822,7 @@
         <v>6300</v>
       </c>
       <c r="B1234" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="C1234">
         <v>131110.69662485569</v>
@@ -17819,7 +17833,7 @@
         <v>6400</v>
       </c>
       <c r="B1235" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="C1235">
         <v>247904.98470651489</v>
@@ -17830,7 +17844,7 @@
         <v>6500</v>
       </c>
       <c r="B1236" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="C1236">
         <v>227403.39012931151</v>
@@ -17841,7 +17855,7 @@
         <v>6600</v>
       </c>
       <c r="B1237" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="C1237">
         <v>426705.61231235729</v>
@@ -17852,7 +17866,7 @@
         <v>6700</v>
       </c>
       <c r="B1238" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="C1238">
         <v>111204.9503292286</v>
@@ -17863,7 +17877,7 @@
         <v>6800</v>
       </c>
       <c r="B1239" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="C1239">
         <v>134910.48330938679</v>
@@ -17874,7 +17888,7 @@
         <v>6900</v>
       </c>
       <c r="B1240" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="C1240">
         <v>223557.46031186369</v>
@@ -17885,7 +17899,7 @@
         <v>7000</v>
       </c>
       <c r="B1241" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="C1241">
         <v>190214.03122162769</v>
@@ -17896,7 +17910,7 @@
         <v>7100</v>
       </c>
       <c r="B1242" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="C1242">
         <v>357067.59984838741</v>
@@ -17907,7 +17921,7 @@
         <v>7200</v>
       </c>
       <c r="B1243" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="C1243">
         <v>99227.798002591517</v>
@@ -17918,7 +17932,7 @@
         <v>7300</v>
       </c>
       <c r="B1244" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="C1244">
         <v>165487.3306477915</v>
@@ -17929,7 +17943,7 @@
         <v>7400</v>
       </c>
       <c r="B1245" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="C1245">
         <v>561894.96064241452</v>
@@ -17940,7 +17954,7 @@
         <v>7500</v>
       </c>
       <c r="B1246" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="C1246">
         <v>70777.547224695227</v>
@@ -17951,7 +17965,7 @@
         <v>7600</v>
       </c>
       <c r="B1247" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="C1247">
         <v>120979.2696148862</v>
@@ -17962,7 +17976,7 @@
         <v>7700</v>
       </c>
       <c r="B1248" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="C1248">
         <v>138507.6414537185</v>
@@ -17973,7 +17987,7 @@
         <v>7800</v>
       </c>
       <c r="B1249" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="C1249">
         <v>97941.808950434992</v>
@@ -17984,7 +17998,7 @@
         <v>7900</v>
       </c>
       <c r="B1250" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="C1250">
         <v>565331.62093312293</v>
@@ -17995,7 +18009,7 @@
         <v>8000</v>
       </c>
       <c r="B1251" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="C1251">
         <v>84155.043324195431</v>
@@ -18006,7 +18020,7 @@
         <v>8200</v>
       </c>
       <c r="B1252" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="C1252">
         <v>112210.0681375444</v>
@@ -18017,7 +18031,7 @@
         <v>8300</v>
       </c>
       <c r="B1253" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="C1253">
         <v>569207.64409812505</v>
@@ -18028,7 +18042,7 @@
         <v>8400</v>
       </c>
       <c r="B1254" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="C1254">
         <v>330292.54541768401</v>
@@ -18039,7 +18053,7 @@
         <v>8500</v>
       </c>
       <c r="B1255" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="C1255">
         <v>176166.45658325031</v>
@@ -18050,7 +18064,7 @@
         <v>8600</v>
       </c>
       <c r="B1256" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="C1256">
         <v>370872.42148315947</v>
@@ -18061,7 +18075,7 @@
         <v>8700</v>
       </c>
       <c r="B1257" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="C1257">
         <v>197189.6691847294</v>
@@ -18072,7 +18086,7 @@
         <v>8800</v>
       </c>
       <c r="B1258" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="C1258">
         <v>88267.800823291924</v>
@@ -18083,7 +18097,7 @@
         <v>8900</v>
       </c>
       <c r="B1259" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="C1259">
         <v>74196.151506871043</v>
@@ -18094,7 +18108,7 @@
         <v>9000</v>
       </c>
       <c r="B1260" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="C1260">
         <v>459244.54591130657</v>
@@ -18105,7 +18119,7 @@
         <v>9100</v>
       </c>
       <c r="B1261" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="C1261">
         <v>153991.67188202421</v>
@@ -18116,7 +18130,7 @@
         <v>9200</v>
       </c>
       <c r="B1262" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="C1262">
         <v>43234.109319770461</v>
@@ -18127,7 +18141,7 @@
         <v>9300</v>
       </c>
       <c r="B1263" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="C1263">
         <v>53315.380750482604</v>
@@ -18138,7 +18152,7 @@
         <v>9400</v>
       </c>
       <c r="B1264" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="C1264">
         <v>67854.480065581287</v>
@@ -18149,7 +18163,7 @@
         <v>9500</v>
       </c>
       <c r="B1265" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="C1265">
         <v>101159.7909155817</v>
@@ -18160,7 +18174,7 @@
         <v>9600</v>
       </c>
       <c r="B1266" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="C1266">
         <v>99121.468174566093</v>
@@ -18171,7 +18185,7 @@
         <v>9700</v>
       </c>
       <c r="B1267" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C1267">
         <v>140810.78565321249</v>
@@ -18182,7 +18196,7 @@
         <v>9800</v>
       </c>
       <c r="B1268" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="C1268">
         <v>33132.775657355407</v>

</xml_diff>